<commit_message>
Organization column added to test files
</commit_message>
<xml_diff>
--- a/test_files/Code_list_incorrect_classification_value.xlsx
+++ b/test_files/Code_list_incorrect_classification_value.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="Codes" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="yti">CodeSchemes!$A$1:$W$2</definedName>
+    <definedName localSheetId="0" name="yti">CodeSchemes!$A$1:$X$2</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -37,15 +37,57 @@
     <t>PREFLABEL_SV</t>
   </si>
   <si>
+    <t>PREFLABEL_EN</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_FI</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_SV</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_EN</t>
+  </si>
+  <si>
+    <t>SHORTNAME</t>
+  </si>
+  <si>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>testikoodi01</t>
+  </si>
+  <si>
+    <t>DRAFT</t>
+  </si>
+  <si>
+    <t>Testikoodi 01</t>
+  </si>
+  <si>
+    <t>Kuvaus</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ORGANIZATION</t>
+  </si>
+  <si>
+    <t>testikoodi02</t>
+  </si>
+  <si>
+    <t>Testikoodi 02</t>
+  </si>
+  <si>
     <t>CLASSIFICATION</t>
   </si>
   <si>
     <t>VERSION</t>
   </si>
   <si>
-    <t>PREFLABEL_EN</t>
-  </si>
-  <si>
     <t>DEFINITION_FI</t>
   </si>
   <si>
@@ -55,15 +97,6 @@
     <t>DEFINITION_EN</t>
   </si>
   <si>
-    <t>DESCRIPTION_FI</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_SV</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_EN</t>
-  </si>
-  <si>
     <t>CHANGENOTE_FI</t>
   </si>
   <si>
@@ -73,12 +106,6 @@
     <t>CHANGENOTE_EN</t>
   </si>
   <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>SOURCE</t>
   </si>
   <si>
@@ -94,88 +121,67 @@
     <t>Koodisto1000</t>
   </si>
   <si>
+    <t>testikoodi03</t>
+  </si>
+  <si>
+    <t>Testikoodi 03</t>
+  </si>
+  <si>
+    <t>testikoodi04</t>
+  </si>
+  <si>
+    <t>Testikoodi 04</t>
+  </si>
+  <si>
+    <t>testikoodi05</t>
+  </si>
+  <si>
+    <t>Testikoodi 05</t>
+  </si>
+  <si>
+    <t>testikoodi06</t>
+  </si>
+  <si>
+    <t>Testikoodi 06</t>
+  </si>
+  <si>
+    <t>testikoodi07</t>
+  </si>
+  <si>
+    <t>Testikoodi 07</t>
+  </si>
+  <si>
+    <t>74a41211-8c99-4835-a519-7a61612b1098</t>
+  </si>
+  <si>
+    <t>testikoodi08</t>
+  </si>
+  <si>
+    <t>Testikoodi 08</t>
+  </si>
+  <si>
+    <t>testikoodi09</t>
+  </si>
+  <si>
+    <t>Testikoodi 09</t>
+  </si>
+  <si>
     <t>P1.2</t>
   </si>
   <si>
-    <t>DRAFT</t>
+    <t>testikoodi10</t>
+  </si>
+  <si>
+    <t>Testikoodi 10</t>
   </si>
   <si>
     <t>koodisto1000</t>
   </si>
   <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
-    <t>testikoodi01</t>
-  </si>
-  <si>
-    <t>Testikoodi 01</t>
-  </si>
-  <si>
-    <t>Kuvaus</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Määritelmä</t>
   </si>
   <si>
     <t>Definition</t>
-  </si>
-  <si>
-    <t>testikoodi02</t>
-  </si>
-  <si>
-    <t>Testikoodi 02</t>
-  </si>
-  <si>
-    <t>testikoodi03</t>
-  </si>
-  <si>
-    <t>Testikoodi 03</t>
-  </si>
-  <si>
-    <t>testikoodi04</t>
-  </si>
-  <si>
-    <t>Testikoodi 04</t>
-  </si>
-  <si>
-    <t>testikoodi05</t>
-  </si>
-  <si>
-    <t>Testikoodi 05</t>
-  </si>
-  <si>
-    <t>testikoodi06</t>
-  </si>
-  <si>
-    <t>Testikoodi 06</t>
-  </si>
-  <si>
-    <t>testikoodi07</t>
-  </si>
-  <si>
-    <t>Testikoodi 07</t>
-  </si>
-  <si>
-    <t>testikoodi08</t>
-  </si>
-  <si>
-    <t>Testikoodi 08</t>
-  </si>
-  <si>
-    <t>testikoodi09</t>
-  </si>
-  <si>
-    <t>Testikoodi 09</t>
-  </si>
-  <si>
-    <t>testikoodi10</t>
-  </si>
-  <si>
-    <t>Testikoodi 10</t>
   </si>
 </sst>
 </file>
@@ -193,6 +199,10 @@
     </font>
     <font/>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <name val="Arial"/>
     </font>
@@ -200,10 +210,6 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -233,38 +239,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -292,192 +283,173 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.67"/>
-    <col customWidth="1" min="2" max="2" width="7.33"/>
-    <col customWidth="1" min="3" max="3" width="14.11"/>
-    <col customWidth="1" min="4" max="4" width="8.33"/>
-    <col customWidth="1" min="5" max="5" width="7.33"/>
-    <col customWidth="1" min="6" max="6" width="15.33"/>
-    <col customWidth="1" min="7" max="7" width="13.0"/>
-    <col customWidth="1" min="8" max="8" width="18.11"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="13.67"/>
-    <col customWidth="1" min="11" max="11" width="13.78"/>
-    <col customWidth="1" min="12" max="12" width="14.33"/>
-    <col customWidth="1" min="13" max="13" width="15.0"/>
-    <col customWidth="1" min="14" max="14" width="15.33"/>
-    <col customWidth="1" min="15" max="15" width="15.0"/>
-    <col customWidth="1" min="16" max="16" width="15.67"/>
-    <col customWidth="1" min="17" max="17" width="15.78"/>
-    <col customWidth="1" min="18" max="18" width="10.67"/>
-    <col customWidth="1" min="19" max="19" width="9.0"/>
-    <col customWidth="1" min="20" max="20" width="11.33"/>
-    <col customWidth="1" min="21" max="21" width="10.33"/>
-    <col customWidth="1" min="22" max="22" width="18.33"/>
-    <col customWidth="1" min="23" max="23" width="7.67"/>
-    <col customWidth="1" min="24" max="26" width="10.56"/>
+    <col customWidth="1" min="1" max="2" width="12.67"/>
+    <col customWidth="1" min="3" max="3" width="7.33"/>
+    <col customWidth="1" min="4" max="4" width="14.11"/>
+    <col customWidth="1" min="5" max="5" width="8.33"/>
+    <col customWidth="1" min="6" max="6" width="7.33"/>
+    <col customWidth="1" min="7" max="7" width="15.33"/>
+    <col customWidth="1" min="8" max="8" width="13.0"/>
+    <col customWidth="1" min="9" max="9" width="18.11"/>
+    <col customWidth="1" min="10" max="10" width="13.0"/>
+    <col customWidth="1" min="11" max="11" width="13.67"/>
+    <col customWidth="1" min="12" max="12" width="13.78"/>
+    <col customWidth="1" min="13" max="13" width="14.33"/>
+    <col customWidth="1" min="14" max="14" width="15.0"/>
+    <col customWidth="1" min="15" max="15" width="15.33"/>
+    <col customWidth="1" min="16" max="16" width="15.0"/>
+    <col customWidth="1" min="17" max="17" width="15.67"/>
+    <col customWidth="1" min="18" max="18" width="15.78"/>
+    <col customWidth="1" min="19" max="19" width="10.67"/>
+    <col customWidth="1" min="20" max="20" width="9.0"/>
+    <col customWidth="1" min="21" max="21" width="11.33"/>
+    <col customWidth="1" min="22" max="22" width="10.33"/>
+    <col customWidth="1" min="23" max="23" width="18.33"/>
+    <col customWidth="1" min="24" max="24" width="7.67"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
       <c r="U1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="V1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="W1" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="X1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2">
         <v>1.0</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="6">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="1">
         <v>43194.0</v>
       </c>
-      <c r="S2" s="6">
+      <c r="T2" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="3"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="1"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-      <c r="I5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="F6" s="11"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -1501,14 +1473,14 @@
     <col customWidth="1" min="9" max="9" width="14.44"/>
     <col customWidth="1" min="10" max="10" width="14.78"/>
     <col customWidth="1" min="11" max="11" width="21.89"/>
-    <col customWidth="1" min="12" max="28" width="10.56"/>
+    <col customWidth="1" min="12" max="14" width="10.56"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1517,7 +1489,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1527,303 +1499,275 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="6">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1">
         <v>43194.0</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="7">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="7">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M5" s="7">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="7">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="7">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="7">
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="7">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M10" s="7">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M11" s="7">
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="3">
         <v>43194.0</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="1">
         <v>47735.0</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>

</xml_diff>